<commit_message>
Working on cleaning up and commenting files
</commit_message>
<xml_diff>
--- a/Officially Used Data/classification_reports.xlsx
+++ b/Officially Used Data/classification_reports.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotan\SchoolStuffs\2024-25\BachelorProject\Openstreetmap_Random_Forest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotan\SchoolStuffs\2024-25\BachelorProject\Openstreetmap_Random_Forest\Officially Used Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E83EB9-C6EE-4040-BE53-0D48ABA52A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B6504A-A6F4-4425-8D3B-9193441C1C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="randomforest1_report" sheetId="1" r:id="rId1"/>
@@ -2476,7 +2476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G338" workbookViewId="0">
+    <sheetView topLeftCell="K209" workbookViewId="0">
       <selection activeCell="AB354" sqref="AB354"/>
     </sheetView>
   </sheetViews>
@@ -8984,6 +8984,18 @@
   </sheetData>
   <conditionalFormatting sqref="B1:D349">
     <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFE67C73"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FF57BB8A"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B352:D354">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.6"/>
@@ -9006,8 +9018,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H352:J354">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFE67C73"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FF57BB8A"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N347:P349">
     <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFE67C73"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FF57BB8A"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N352:P354">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.6"/>
@@ -9030,8 +9066,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z347:AB349">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="T352:V354">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.6"/>
@@ -9042,44 +9078,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B352:D354">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.6"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFE67C73"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FF57BB8A"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H352:J354">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.6"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFE67C73"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FF57BB8A"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N352:P354">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.6"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFE67C73"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FF57BB8A"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T352:V354">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="Z347:AB349">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.6"/>
@@ -15088,8 +15088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7156E14-7211-43D3-A5D3-F349E032C643}">
   <dimension ref="A1:E315"/>
   <sheetViews>
-    <sheetView topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="D315" sqref="D315"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>